<commit_message>
Array formula & keep CR_LF & 3D example (sheets, columns & rows)
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_demo_021-xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_demo_021-xlsx.w3mi.data.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moldab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\!current\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50987295-3BAD-4289-877E-78174E491290}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formula" sheetId="2" r:id="rId1"/>
     <sheet name="SimpleTree" sheetId="3" r:id="rId2"/>
-    <sheet name="Tree3" sheetId="4" r:id="rId3"/>
+    <sheet name="ArrayFormula" sheetId="5" r:id="rId3"/>
+    <sheet name="Tree3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="ARR_NUMBER">ArrayFormula!$D$5</definedName>
+    <definedName name="ARR_SUM1">ArrayFormula!$E$5</definedName>
     <definedName name="E_">Tree3!$E$6</definedName>
     <definedName name="F_">SimpleTree!$F$5</definedName>
     <definedName name="RANGE_SUM1" localSheetId="1">SimpleTree!$E$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>{R-T-SUM2}</t>
   </si>
@@ -109,13 +113,37 @@
   </si>
   <si>
     <t>{R-T;group=GROUP}</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Array FM1</t>
+  </si>
+  <si>
+    <t>Array FM2</t>
+  </si>
+  <si>
+    <t>Ordinary FM (error)</t>
+  </si>
+  <si>
+    <t>Number * SUM 1</t>
+  </si>
+  <si>
+    <t>Totals with additional column</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>After</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +174,20 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -167,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -283,12 +325,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -366,6 +432,38 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -378,9 +476,310 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -391,6 +790,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ARR_TAB" displayName="ARR_TAB" ref="B4:F6" totalsRowCount="1" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
+  <autoFilter ref="B4:F5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Caption" totalsRowLabel="Totals with additional column" dataDxfId="9" totalsRowDxfId="4" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Group" dataDxfId="8" totalsRowDxfId="3" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Number" dataDxfId="7" totalsRowDxfId="2" dataCellStyle="Normal 2">
+      <calculatedColumnFormula>CODE(RIGHT(ARR_TAB[Group],1))-64</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="SUM 1" dataDxfId="6" totalsRowDxfId="1" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Number * SUM 1" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="0" dataCellStyle="Normal 2">
+      <calculatedColumnFormula>ARR_TAB[Number]*ARR_TAB[SUM 1]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -655,7 +1072,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -696,11 +1113,11 @@
       <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -745,11 +1162,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +1268,133 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="19.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="39" t="e">
+        <f>SUM(ARR_TAB[Number]*ARR_TAB[SUM 1])</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="39" t="e">
+        <f t="array" ref="C2">SUM(ARR_TAB[Number]*ARR_TAB[SUM 1])</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="39" t="e">
+        <f t="array" ref="C3">SUM(ARR_NUMBER*ARR_SUM1)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="31">
+        <f>CODE(RIGHT(ARR_TAB[Group],1))-64</f>
+        <v>61</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="36" t="e">
+        <f>ARR_TAB[Number]*ARR_TAB[SUM 1]</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38" t="e">
+        <f>SUBTOTAL(109,ARR_TAB[Number * SUM 1])</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="39" t="e">
+        <f t="array" ref="C8">SUM(ARR_TAB[Number]*ARR_TAB[SUM 1])</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="39" t="e">
+        <f t="array" ref="C9">SUM(ARR_NUMBER*ARR_SUM1)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>